<commit_message>
fixing model input, e.g. age^2, individual items, scaling
still open questions about scaling
</commit_message>
<xml_diff>
--- a/Yerkes/Drew version/persAlignments.xlsx
+++ b/Yerkes/Drew version/persAlignments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="144">
   <si>
     <t xml:space="preserve">Outgoing       .         </t>
   </si>
@@ -309,13 +309,160 @@
   </si>
   <si>
     <t>Imitative     -0.06066352</t>
+  </si>
+  <si>
+    <t>(Intercept)    0.0628444918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sex            .           </t>
+  </si>
+  <si>
+    <t>age            0.0430165272</t>
+  </si>
+  <si>
+    <t>age2           0.1117059672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depressed      .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fearful        .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Persistent     .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cautious       .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stable         .           </t>
+  </si>
+  <si>
+    <t>Autistic      -0.0473130008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stingy         .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jealous        .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reckless       .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sociable       .           </t>
+  </si>
+  <si>
+    <t>Timid         -0.0142789320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sympathetic    .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Playful        .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solitary       .           </t>
+  </si>
+  <si>
+    <t>Active        -0.0974213317</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helpful        .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bullying       .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aggressive     .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipiulative  .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gentle         .           </t>
+  </si>
+  <si>
+    <t>Affectionate   0.0266638768</t>
+  </si>
+  <si>
+    <t>Excitable     -0.0000547059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impulsive      .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inquisitve     .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submissive     .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent      .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Irritible      .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Predictable    .           </t>
+  </si>
+  <si>
+    <t>Decisive       0.0499958689</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Independent    .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensitive      .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defiant        .           </t>
+  </si>
+  <si>
+    <t>Intelligent    0.0268132986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protective     .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inventive      .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clumsy         .           </t>
+  </si>
+  <si>
+    <t>Erratic       -0.0282228804</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Friendly       .           </t>
+  </si>
+  <si>
+    <t>Lazy           0.1134626736</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disorganized   .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unemotional    .           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imitative      .           </t>
+  </si>
+  <si>
+    <t>Dominant       0.0344058377</t>
+  </si>
+  <si>
+    <t>CORRECT FOR MEDICATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age2           .         </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,6 +475,14 @@
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -350,11 +505,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,15 +791,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -653,8 +809,18 @@
       <c r="I1" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="S1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -664,8 +830,14 @@
       <c r="I2" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -675,8 +847,14 @@
       <c r="I3" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,8 +864,14 @@
       <c r="M4" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
@@ -697,8 +881,14 @@
       <c r="M5" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -711,8 +901,14 @@
       <c r="M6" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -725,8 +921,14 @@
       <c r="M7" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -736,8 +938,14 @@
       <c r="I8" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -750,8 +958,14 @@
       <c r="M9" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
@@ -761,8 +975,14 @@
       <c r="I10" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>48</v>
       </c>
@@ -775,16 +995,28 @@
       <c r="M11" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -794,8 +1026,14 @@
       <c r="M13" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -805,8 +1043,14 @@
       <c r="M14" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -816,16 +1060,28 @@
       <c r="M15" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -838,24 +1094,42 @@
       <c r="M17" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S17" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -865,8 +1139,14 @@
       <c r="I20" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S20" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -879,8 +1159,14 @@
       <c r="M21" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S21" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -893,8 +1179,14 @@
       <c r="M22" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -904,8 +1196,14 @@
       <c r="M23" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
@@ -918,8 +1216,14 @@
       <c r="M24" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S24" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -932,8 +1236,14 @@
       <c r="M25" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -946,8 +1256,14 @@
       <c r="M26" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -960,16 +1276,28 @@
       <c r="M27" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="X27" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="X28" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -982,8 +1310,14 @@
       <c r="M29" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S29" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="X29" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>17</v>
       </c>
@@ -993,8 +1327,14 @@
       <c r="M30" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S30" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="X30" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
@@ -1004,8 +1344,14 @@
       <c r="I31" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S31" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="X31" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>18</v>
       </c>
@@ -1015,8 +1361,14 @@
       <c r="I32" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="X32" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -1029,38 +1381,108 @@
       <c r="M33" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S33" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="X33" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S34" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="X34" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S35" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="X35" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S36" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S37" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S38" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I39" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S39" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I40" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S40" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I41" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S41" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S42" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S43" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I44" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S44" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I45" s="1" t="s">
         <v>94</v>
+      </c>
+      <c r="S45" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S46" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S47" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>